<commit_message>
Working through a lot of snippets to figure out the best way to update excel data for embedded powerpoint charts
</commit_message>
<xml_diff>
--- a/Practice2.xlsx
+++ b/Practice2.xlsx
@@ -3,10 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-32340" yWindow="8420" windowWidth="28040" windowHeight="17440" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="17920" windowHeight="21900" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2 (2)" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -16,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -26,12 +28,8 @@
     </font>
     <font>
       <name val="Calibri"/>
-      <family val="2"/>
       <b val="1"/>
       <sz val="12"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -42,7 +40,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -65,22 +63,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -460,10 +449,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -474,158 +463,38 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>New Column -1</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>New Column</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>NewColumnAgain4</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>NewColumnAgain5</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>NewColumnAgain6</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>Column</t>
-        </is>
-      </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>Column1</t>
-        </is>
-      </c>
-      <c r="F1" s="2" t="inlineStr">
-        <is>
-          <t>Column2</t>
-        </is>
-      </c>
-      <c r="G1" s="2" t="inlineStr">
-        <is>
-          <t>Column3</t>
-        </is>
-      </c>
-      <c r="H1" s="2" t="inlineStr">
-        <is>
-          <t>Column4</t>
-        </is>
-      </c>
-      <c r="I1" s="2" t="inlineStr">
-        <is>
-          <t>Column5</t>
-        </is>
-      </c>
-      <c r="J1" s="2" t="inlineStr">
-        <is>
-          <t>Column6</t>
-        </is>
-      </c>
-      <c r="K1" s="2" t="inlineStr">
-        <is>
-          <t>Column7</t>
-        </is>
-      </c>
-      <c r="L1" s="2" t="inlineStr">
-        <is>
-          <t>Column8</t>
-        </is>
-      </c>
-      <c r="M1" s="2" t="inlineStr">
-        <is>
-          <t>Column9</t>
-        </is>
-      </c>
-      <c r="N1" s="2" t="inlineStr">
-        <is>
-          <t>Column10</t>
-        </is>
-      </c>
-      <c r="O1" s="2" t="inlineStr">
-        <is>
-          <t>Column11</t>
-        </is>
-      </c>
-      <c r="P1" s="2" t="inlineStr">
-        <is>
-          <t>Column12</t>
-        </is>
-      </c>
-      <c r="Q1" s="2" t="inlineStr">
-        <is>
-          <t>Column13</t>
-        </is>
-      </c>
-      <c r="R1" s="2" t="inlineStr">
-        <is>
-          <t>Column14</t>
-        </is>
-      </c>
-      <c r="S1" s="2" t="inlineStr">
-        <is>
-          <t>Column15</t>
-        </is>
-      </c>
-      <c r="T1" s="2" t="inlineStr">
-        <is>
-          <t>Column16</t>
-        </is>
-      </c>
-      <c r="U1" s="2" t="inlineStr">
-        <is>
-          <t>Column17</t>
-        </is>
-      </c>
-      <c r="V1" s="2" t="inlineStr">
-        <is>
-          <t>Column18</t>
-        </is>
-      </c>
-      <c r="W1" s="2" t="inlineStr">
-        <is>
-          <t>Column19</t>
-        </is>
-      </c>
-      <c r="X1" s="2" t="inlineStr">
-        <is>
-          <t>Column20</t>
-        </is>
-      </c>
-      <c r="Y1" s="2" t="inlineStr">
-        <is>
-          <t>Column21</t>
-        </is>
-      </c>
-      <c r="Z1" s="2" t="inlineStr">
-        <is>
-          <t>Column22</t>
-        </is>
-      </c>
-      <c r="AA1" s="2" t="inlineStr">
-        <is>
-          <t>Column23</t>
-        </is>
-      </c>
-      <c r="AB1" s="2" t="inlineStr">
-        <is>
-          <t>Column24</t>
-        </is>
-      </c>
-      <c r="AC1" s="2" t="inlineStr">
-        <is>
-          <t>Column25</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
         <v>10</v>
@@ -634,87 +503,15 @@
         <v>10</v>
       </c>
       <c r="E2" t="n">
-        <v>10</v>
-      </c>
-      <c r="F2" t="n">
-        <v>10</v>
-      </c>
-      <c r="G2" t="n">
-        <v>10</v>
-      </c>
-      <c r="H2" t="n">
-        <v>10</v>
-      </c>
-      <c r="I2" t="n">
-        <v>10</v>
-      </c>
-      <c r="J2" t="n">
-        <v>10</v>
-      </c>
-      <c r="K2" t="n">
-        <v>10</v>
-      </c>
-      <c r="L2" t="n">
-        <v>10</v>
-      </c>
-      <c r="M2" t="n">
-        <v>10</v>
-      </c>
-      <c r="N2" t="n">
-        <v>10</v>
-      </c>
-      <c r="O2" t="n">
-        <v>10</v>
-      </c>
-      <c r="P2" t="n">
-        <v>10</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>10</v>
-      </c>
-      <c r="R2" t="n">
-        <v>10</v>
-      </c>
-      <c r="S2" t="n">
-        <v>10</v>
-      </c>
-      <c r="T2" t="n">
-        <v>10</v>
-      </c>
-      <c r="U2" t="n">
-        <v>10</v>
-      </c>
-      <c r="V2" t="n">
-        <v>10</v>
-      </c>
-      <c r="W2" t="n">
-        <v>10</v>
-      </c>
-      <c r="X2" t="n">
-        <v>10</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>10</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>10</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>10</v>
-      </c>
-      <c r="AB2" t="n">
-        <v>10</v>
-      </c>
-      <c r="AC2" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="C3" t="n">
         <v>20</v>
@@ -723,87 +520,15 @@
         <v>20</v>
       </c>
       <c r="E3" t="n">
-        <v>20</v>
-      </c>
-      <c r="F3" t="n">
-        <v>20</v>
-      </c>
-      <c r="G3" t="n">
-        <v>20</v>
-      </c>
-      <c r="H3" t="n">
-        <v>20</v>
-      </c>
-      <c r="I3" t="n">
-        <v>20</v>
-      </c>
-      <c r="J3" t="n">
-        <v>20</v>
-      </c>
-      <c r="K3" t="n">
-        <v>20</v>
-      </c>
-      <c r="L3" t="n">
-        <v>20</v>
-      </c>
-      <c r="M3" t="n">
-        <v>20</v>
-      </c>
-      <c r="N3" t="n">
-        <v>20</v>
-      </c>
-      <c r="O3" t="n">
-        <v>20</v>
-      </c>
-      <c r="P3" t="n">
-        <v>20</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>20</v>
-      </c>
-      <c r="R3" t="n">
-        <v>20</v>
-      </c>
-      <c r="S3" t="n">
-        <v>20</v>
-      </c>
-      <c r="T3" t="n">
-        <v>20</v>
-      </c>
-      <c r="U3" t="n">
-        <v>20</v>
-      </c>
-      <c r="V3" t="n">
-        <v>20</v>
-      </c>
-      <c r="W3" t="n">
-        <v>20</v>
-      </c>
-      <c r="X3" t="n">
-        <v>20</v>
-      </c>
-      <c r="Y3" t="n">
-        <v>20</v>
-      </c>
-      <c r="Z3" t="n">
-        <v>20</v>
-      </c>
-      <c r="AA3" t="n">
-        <v>20</v>
-      </c>
-      <c r="AB3" t="n">
-        <v>20</v>
-      </c>
-      <c r="AC3" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="C4" t="n">
         <v>30</v>
@@ -814,80 +539,167 @@
       <c r="E4" t="n">
         <v>30</v>
       </c>
-      <c r="F4" t="n">
-        <v>30</v>
-      </c>
-      <c r="G4" t="n">
-        <v>30</v>
-      </c>
-      <c r="H4" t="n">
-        <v>30</v>
-      </c>
-      <c r="I4" t="n">
-        <v>30</v>
-      </c>
-      <c r="J4" t="n">
-        <v>30</v>
-      </c>
-      <c r="K4" t="n">
-        <v>30</v>
-      </c>
-      <c r="L4" t="n">
-        <v>30</v>
-      </c>
-      <c r="M4" t="n">
-        <v>30</v>
-      </c>
-      <c r="N4" t="n">
-        <v>30</v>
-      </c>
-      <c r="O4" t="n">
-        <v>30</v>
-      </c>
-      <c r="P4" t="n">
-        <v>30</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>30</v>
-      </c>
-      <c r="R4" t="n">
-        <v>30</v>
-      </c>
-      <c r="S4" t="n">
-        <v>30</v>
-      </c>
-      <c r="T4" t="n">
-        <v>30</v>
-      </c>
-      <c r="U4" t="n">
-        <v>30</v>
-      </c>
-      <c r="V4" t="n">
-        <v>30</v>
-      </c>
-      <c r="W4" t="n">
-        <v>30</v>
-      </c>
-      <c r="X4" t="n">
-        <v>30</v>
-      </c>
-      <c r="Y4" t="n">
-        <v>30</v>
-      </c>
-      <c r="Z4" t="n">
-        <v>30</v>
-      </c>
-      <c r="AA4" t="n">
-        <v>30</v>
-      </c>
-      <c r="AB4" t="n">
-        <v>30</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>30</v>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <cols>
+    <col width="19.5" customWidth="1" min="1" max="1"/>
+    <col width="18.1640625" customWidth="1" min="2" max="2"/>
+    <col width="21.5" customWidth="1" min="3" max="3"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>NewColumnAgain4</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>NewColumnAgain5</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>NewColumnAgain6</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>10</v>
+      </c>
+      <c r="B2" t="n">
+        <v>10</v>
+      </c>
+      <c r="C2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>20</v>
+      </c>
+      <c r="B3" t="n">
+        <v>20</v>
+      </c>
+      <c r="C3" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>30</v>
+      </c>
+      <c r="B4" t="n">
+        <v>30</v>
+      </c>
+      <c r="C4" t="n">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>NewColumnAgain4</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>NewColumnAgain5</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>NewColumnAgain6</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>10</v>
+      </c>
+      <c r="B2" t="n">
+        <v>10</v>
+      </c>
+      <c r="C2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>20</v>
+      </c>
+      <c r="B3" t="n">
+        <v>20</v>
+      </c>
+      <c r="C3" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>30</v>
+      </c>
+      <c r="B4" t="n">
+        <v>30</v>
+      </c>
+      <c r="C4" t="n">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add new columns of data to existing worksheet is working correctly
</commit_message>
<xml_diff>
--- a/Practice2.xlsx
+++ b/Practice2.xlsx
@@ -3,11 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="17920" windowHeight="21900" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-24420" yWindow="6300" windowWidth="17920" windowHeight="21100" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2 (2)" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet 2 copy" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
@@ -28,6 +28,7 @@
     </font>
     <font>
       <name val="Calibri"/>
+      <family val="2"/>
       <b val="1"/>
       <sz val="12"/>
     </font>
@@ -449,10 +450,211 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <cols>
+    <col width="19.5" customWidth="1" min="1" max="1"/>
+    <col width="18.1640625" customWidth="1" min="2" max="2"/>
+    <col width="21.5" customWidth="1" min="3" max="3"/>
+    <col width="30.6640625" customWidth="1" min="4" max="4"/>
+    <col width="18.83203125" customWidth="1" min="5" max="5"/>
+    <col width="21.5" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Old Column</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>New Column D</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>New Column C</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>New Column B</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>New Column A</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Old 2</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Old 3</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Old 4</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Old 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="n">
+        <v>10</v>
+      </c>
+      <c r="H2" t="n">
+        <v>10</v>
+      </c>
+      <c r="I2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" t="n">
+        <v>20</v>
+      </c>
+      <c r="H3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I3" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" t="n">
+        <v>3</v>
+      </c>
+      <c r="G4" t="n">
+        <v>30</v>
+      </c>
+      <c r="H4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I4" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>5</v>
+      </c>
+      <c r="C5" t="n">
+        <v>5</v>
+      </c>
+      <c r="D5" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" t="n">
+        <v>4</v>
+      </c>
+      <c r="F5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>6</v>
+      </c>
+      <c r="C6" t="n">
+        <v>6</v>
+      </c>
+      <c r="D6" t="n">
+        <v>5</v>
+      </c>
+      <c r="E6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F6" t="n">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -465,27 +667,32 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>New Column -1</t>
+          <t>Old 1</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>New Column</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>NewColumnAgain4</t>
+          <t>New Column A</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Old 2</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>NewColumnAgain5</t>
+          <t>Old 3</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>NewColumnAgain6</t>
+          <t>Old 4</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Old 5</t>
         </is>
       </c>
     </row>
@@ -497,12 +704,15 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
         <v>10</v>
       </c>
       <c r="E2" t="n">
+        <v>10</v>
+      </c>
+      <c r="F2" t="n">
         <v>10</v>
       </c>
     </row>
@@ -514,12 +724,15 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="D3" t="n">
         <v>20</v>
       </c>
       <c r="E3" t="n">
+        <v>20</v>
+      </c>
+      <c r="F3" t="n">
         <v>20</v>
       </c>
     </row>
@@ -531,12 +744,15 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="D4" t="n">
         <v>30</v>
       </c>
       <c r="E4" t="n">
+        <v>30</v>
+      </c>
+      <c r="F4" t="n">
         <v>30</v>
       </c>
     </row>
@@ -547,6 +763,9 @@
       <c r="B5" t="n">
         <v>4</v>
       </c>
+      <c r="C5" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -555,79 +774,8 @@
       <c r="B6" t="n">
         <v>5</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
-  <cols>
-    <col width="19.5" customWidth="1" min="1" max="1"/>
-    <col width="18.1640625" customWidth="1" min="2" max="2"/>
-    <col width="21.5" customWidth="1" min="3" max="3"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>NewColumnAgain4</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>NewColumnAgain5</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>NewColumnAgain6</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>10</v>
-      </c>
-      <c r="B2" t="n">
-        <v>10</v>
-      </c>
-      <c r="C2" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>20</v>
-      </c>
-      <c r="B3" t="n">
-        <v>20</v>
-      </c>
-      <c r="C3" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>30</v>
-      </c>
-      <c r="B4" t="n">
-        <v>30</v>
-      </c>
-      <c r="C4" t="n">
-        <v>30</v>
+      <c r="C6" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>